<commit_message>
- added a bit of SPI initialization code - moved SD flush to A12 with it's own EXTI - added 2nd revision board (see revision-history.txt for details)
</commit_message>
<xml_diff>
--- a/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
+++ b/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.gh\robot-corral\mazebot\software\sensors-and-motors\lib-driver-stm32l496ze\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CE0E84-FB66-44EE-9F7C-C66E26171120}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11453D20-B101-45CD-9D2A-090B3987904C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="2" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
   </bookViews>
   <sheets>
     <sheet name="Timers" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>TIM5</t>
   </si>
@@ -107,13 +107,109 @@
   </si>
   <si>
     <t>Right motor encoder B</t>
+  </si>
+  <si>
+    <t>DMA1</t>
+  </si>
+  <si>
+    <t>Channel 1</t>
+  </si>
+  <si>
+    <t>Channel 2</t>
+  </si>
+  <si>
+    <t>Channel 3</t>
+  </si>
+  <si>
+    <t>Channel 4</t>
+  </si>
+  <si>
+    <t>Channel 5</t>
+  </si>
+  <si>
+    <t>Channel 6</t>
+  </si>
+  <si>
+    <t>Channel 7</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>ADC2</t>
+  </si>
+  <si>
+    <t>ADC3</t>
+  </si>
+  <si>
+    <t>USART1_TX</t>
+  </si>
+  <si>
+    <t>USART1_RX</t>
+  </si>
+  <si>
+    <t>USART2_RX</t>
+  </si>
+  <si>
+    <t>USART2_TX</t>
+  </si>
+  <si>
+    <t>DMA2</t>
+  </si>
+  <si>
+    <t>SPI3_TX</t>
+  </si>
+  <si>
+    <t>SPI3_RX</t>
+  </si>
+  <si>
+    <t>SDMMC1</t>
+  </si>
+  <si>
+    <t>I2C1_RX</t>
+  </si>
+  <si>
+    <t>I2C1_TX</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>SPI3 TX</t>
+  </si>
+  <si>
+    <t>SPI3 RX</t>
+  </si>
+  <si>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>Priority 1</t>
+  </si>
+  <si>
+    <t>EXTI_12</t>
+  </si>
+  <si>
+    <t>Shares the same IRQ as EXTI_11</t>
+  </si>
+  <si>
+    <t>Priority 2</t>
+  </si>
+  <si>
+    <t>EXTI_6</t>
+  </si>
+  <si>
+    <t>Start/Pause button</t>
+  </si>
+  <si>
+    <t>Flush SD (will be moved later to EXTI_9)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,13 +225,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -156,15 +264,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -480,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BA5619-4332-443C-8489-BC42719C7856}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -577,37 +703,319 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D00A580-3AA8-4C2E-B4E4-CE8FB552585E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>1</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>2</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>3</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>4</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>5</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>6</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>7</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFD585D-7293-41F5-9BE9-9477187D65E4}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -615,12 +1023,59 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- added line sensor adc code - fixed SPI DMA IRQ handlers to check all flags in one call (as multiple flags can be set)
</commit_message>
<xml_diff>
--- a/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
+++ b/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.gh\robot-corral\mazebot\software\sensors-and-motors\lib-driver-stm32l496ze\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11453D20-B101-45CD-9D2A-090B3987904C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9025513-9413-4128-BA7B-8E8F53C95CAC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="2" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="3" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
   </bookViews>
   <sheets>
     <sheet name="Timers" sheetId="1" r:id="rId1"/>
     <sheet name="DMA" sheetId="2" r:id="rId2"/>
     <sheet name="Interrupt Priorities" sheetId="4" r:id="rId3"/>
+    <sheet name="ADC" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>TIM5</t>
   </si>
@@ -175,12 +176,6 @@
     <t>Request</t>
   </si>
   <si>
-    <t>SPI3 TX</t>
-  </si>
-  <si>
-    <t>SPI3 RX</t>
-  </si>
-  <si>
     <t>IMU</t>
   </si>
   <si>
@@ -203,13 +198,49 @@
   </si>
   <si>
     <t>Flush SD (will be moved later to EXTI_9)</t>
+  </si>
+  <si>
+    <t>Sensor #</t>
+  </si>
+  <si>
+    <t>ADC #</t>
+  </si>
+  <si>
+    <t>ADC Channel #</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>ADC1 DMA Error</t>
+  </si>
+  <si>
+    <t>ADC2 DMA Error</t>
+  </si>
+  <si>
+    <t>Line sensor</t>
+  </si>
+  <si>
+    <t>ADC3 DMA Error</t>
+  </si>
+  <si>
+    <t>SPI3 RX DMA Complete</t>
+  </si>
+  <si>
+    <t>SPI3 TX DMA Complete</t>
+  </si>
+  <si>
+    <t>SPI3 RX DMA Error</t>
+  </si>
+  <si>
+    <t>SPI3 TX DMA Error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +263,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,8 +283,37 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -263,13 +330,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
@@ -288,10 +371,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="3" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -706,7 +794,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,15 +1084,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFD585D-7293-41F5-9BE9-9477187D65E4}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1033,49 +1121,446 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC9F77D-643E-4A1B-A82C-DD5901F583DB}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>55</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
+        <v>12</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10">
+        <v>16</v>
+      </c>
+      <c r="C17" s="10">
+        <v>3</v>
+      </c>
+      <c r="D17" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10">
+        <v>17</v>
+      </c>
+      <c r="C18" s="10">
+        <v>3</v>
+      </c>
+      <c r="D18" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10">
+        <v>18</v>
+      </c>
+      <c r="C19" s="10">
+        <v>3</v>
+      </c>
+      <c r="D19" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10">
+        <v>19</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10">
+        <v>20</v>
+      </c>
+      <c r="C21" s="10">
+        <v>3</v>
+      </c>
+      <c r="D21" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10">
+        <v>21</v>
+      </c>
+      <c r="C22" s="10">
+        <v>3</v>
+      </c>
+      <c r="D22" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10">
+        <v>22</v>
+      </c>
+      <c r="C23" s="10">
+        <v>3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10">
+        <v>23</v>
+      </c>
+      <c r="C24" s="10">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- added async tasks framework - migrated IMU/LineSensor to use task framework (return sampling frequency, still need to calculate actual values)
</commit_message>
<xml_diff>
--- a/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
+++ b/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.gh\robot-corral\mazebot\software\sensors-and-motors\lib-driver-stm32l496ze\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9025513-9413-4128-BA7B-8E8F53C95CAC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA73344F-6165-409A-BF46-396B75EDE515}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="3" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="2" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
   </bookViews>
   <sheets>
     <sheet name="Timers" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>TIM5</t>
   </si>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>SPI3 TX DMA Error</t>
+  </si>
+  <si>
+    <t>TIM2</t>
+  </si>
+  <si>
+    <t>Task scheduling (32 bit)</t>
+  </si>
+  <si>
+    <t>Priority 3</t>
+  </si>
+  <si>
+    <t>Task scheduler timer</t>
   </si>
 </sst>
 </file>
@@ -692,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BA5619-4332-443C-8489-BC42719C7856}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,49 +750,57 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1084,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFD585D-7293-41F5-9BE9-9477187D65E4}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,6 +1226,20 @@
         <v>53</v>
       </c>
     </row>
+    <row r="21" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1215,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC9F77D-643E-4A1B-A82C-DD5901F583DB}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- added code to meazure timing of interrupts, etc. - added code to call IMU/LineSensor start query - added MIN function - SPI now remembers which pin it needs to disable on completion
</commit_message>
<xml_diff>
--- a/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
+++ b/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.gh\robot-corral\mazebot\software\sensors-and-motors\lib-driver-stm32l496ze\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA73344F-6165-409A-BF46-396B75EDE515}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7668375A-41E7-48B9-9978-A13DF659A8E7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="2" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="1" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
   </bookViews>
   <sheets>
     <sheet name="Timers" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>TIM5</t>
   </si>
@@ -143,12 +143,6 @@
     <t>ADC3</t>
   </si>
   <si>
-    <t>USART1_TX</t>
-  </si>
-  <si>
-    <t>USART1_RX</t>
-  </si>
-  <si>
     <t>USART2_RX</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
   </si>
   <si>
     <t>SPI3_RX</t>
-  </si>
-  <si>
-    <t>SDMMC1</t>
   </si>
   <si>
     <t>I2C1_RX</t>
@@ -750,10 +741,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -813,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D00A580-3AA8-4C2E-B4E4-CE8FB552585E}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,7 +825,7 @@
     <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -891,17 +882,13 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -966,13 +953,13 @@
     </row>
     <row r="13" spans="1:8" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>26</v>
@@ -1032,10 +1019,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1065,10 +1052,10 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1090,9 +1077,7 @@
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -1106,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFD585D-7293-41F5-9BE9-9477187D65E4}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -1141,103 +1126,103 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>67</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1263,16 +1248,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- line sensor driver will now calculate displacement (as ADC is quite fast and it is implementation specific) - added status LED code for calibrating/running/paused - added code to compute yaw delta value - moved robot code to lib-robot - added buttons handling code - changed interrupt priorities (buttons now have higher priority)
</commit_message>
<xml_diff>
--- a/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
+++ b/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.gh\robot-corral\mazebot\software\sensors-and-motors\lib-driver-stm32l496ze\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7668375A-41E7-48B9-9978-A13DF659A8E7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438C73D6-2CDF-412A-8A22-A599B33795A3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="1" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="2" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
   </bookViews>
   <sheets>
     <sheet name="Timers" sheetId="1" r:id="rId1"/>
@@ -698,7 +698,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D00A580-3AA8-4C2E-B4E4-CE8FB552585E}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFD585D-7293-41F5-9BE9-9477187D65E4}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1143,72 +1143,72 @@
     <row r="8" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-    </row>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
- added SDMMC headers for STM32L4 - added SD resources to resources map - added code to power up and detect SD card type (SDHC or SDSC) - lowered task timer priority
</commit_message>
<xml_diff>
--- a/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
+++ b/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.gh\robot-corral\mazebot\software\sensors-and-motors\lib-driver-stm32l496ze\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438C73D6-2CDF-412A-8A22-A599B33795A3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C3A793-9E60-419F-BCCB-A3D5729CF4E8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="2" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>TIM5</t>
   </si>
@@ -237,6 +237,21 @@
   </si>
   <si>
     <t>Task scheduler timer</t>
+  </si>
+  <si>
+    <t>SDMMC1</t>
+  </si>
+  <si>
+    <t>Priority 4</t>
+  </si>
+  <si>
+    <t>SDMMC1 DMA</t>
+  </si>
+  <si>
+    <t>EXTI_1</t>
+  </si>
+  <si>
+    <t>SD Detect</t>
   </si>
 </sst>
 </file>
@@ -805,7 +820,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1077,7 +1092,9 @@
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -1089,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFD585D-7293-41F5-9BE9-9477187D65E4}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,54 +1135,54 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="13" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
@@ -1173,7 +1190,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
@@ -1181,7 +1198,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
@@ -1189,15 +1206,15 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>58</v>
@@ -1205,23 +1222,47 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B29" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- added sd read blocks function (working) - moved all SD related state into 1 structure (should do similar for other devices) - fixed resources.xlsx file to properly show rev 1.1 resource usage (DMAs, DMAs priorities)
</commit_message>
<xml_diff>
--- a/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
+++ b/software/sensors-and-motors/lib-driver-stm32l496ze/docs/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.gh\robot-corral\mazebot\software\sensors-and-motors\lib-driver-stm32l496ze\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C3A793-9E60-419F-BCCB-A3D5729CF4E8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D718CB06-3DC8-479E-A6E3-B73AF7EC6997}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" activeTab="2" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12060" xr2:uid="{0728F7C4-FB85-435A-BB7B-5131B6B38990}"/>
   </bookViews>
   <sheets>
     <sheet name="Timers" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>TIM5</t>
   </si>
@@ -53,9 +53,6 @@
     <t>EXTI_0</t>
   </si>
   <si>
-    <t>EXTI_11</t>
-  </si>
-  <si>
     <t>Left motor error (over-current)</t>
   </si>
   <si>
@@ -167,30 +164,15 @@
     <t>Request</t>
   </si>
   <si>
-    <t>IMU</t>
-  </si>
-  <si>
     <t>Priority 1</t>
   </si>
   <si>
-    <t>EXTI_12</t>
-  </si>
-  <si>
-    <t>Shares the same IRQ as EXTI_11</t>
-  </si>
-  <si>
     <t>Priority 2</t>
   </si>
   <si>
-    <t>EXTI_6</t>
-  </si>
-  <si>
     <t>Start/Pause button</t>
   </si>
   <si>
-    <t>Flush SD (will be moved later to EXTI_9)</t>
-  </si>
-  <si>
     <t>Sensor #</t>
   </si>
   <si>
@@ -203,30 +185,9 @@
     <t>#</t>
   </si>
   <si>
-    <t>ADC1 DMA Error</t>
-  </si>
-  <si>
-    <t>ADC2 DMA Error</t>
-  </si>
-  <si>
     <t>Line sensor</t>
   </si>
   <si>
-    <t>ADC3 DMA Error</t>
-  </si>
-  <si>
-    <t>SPI3 RX DMA Complete</t>
-  </si>
-  <si>
-    <t>SPI3 TX DMA Complete</t>
-  </si>
-  <si>
-    <t>SPI3 RX DMA Error</t>
-  </si>
-  <si>
-    <t>SPI3 TX DMA Error</t>
-  </si>
-  <si>
     <t>TIM2</t>
   </si>
   <si>
@@ -236,22 +197,82 @@
     <t>Priority 3</t>
   </si>
   <si>
-    <t>Task scheduler timer</t>
-  </si>
-  <si>
     <t>SDMMC1</t>
   </si>
   <si>
     <t>Priority 4</t>
   </si>
   <si>
-    <t>SDMMC1 DMA</t>
-  </si>
-  <si>
     <t>EXTI_1</t>
   </si>
   <si>
     <t>SD Detect</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>GPI/PD1</t>
+  </si>
+  <si>
+    <t>GPI/PF0</t>
+  </si>
+  <si>
+    <t>GPI/PB11</t>
+  </si>
+  <si>
+    <t>EXTI_9_5</t>
+  </si>
+  <si>
+    <t>EXTI_15_10</t>
+  </si>
+  <si>
+    <t>GPI/PA8</t>
+  </si>
+  <si>
+    <t>SD Flush</t>
+  </si>
+  <si>
+    <t>GPI/PE6</t>
+  </si>
+  <si>
+    <t>IMU RX</t>
+  </si>
+  <si>
+    <t>IMU TX</t>
+  </si>
+  <si>
+    <t>SPI3</t>
+  </si>
+  <si>
+    <t>DMA 2, Channel 2</t>
+  </si>
+  <si>
+    <t>DMA 2, Channel 1</t>
+  </si>
+  <si>
+    <t>DMA 1, Channel 1</t>
+  </si>
+  <si>
+    <t>DMA 1, Channel 2</t>
+  </si>
+  <si>
+    <t>DMA 1, Channel 3</t>
+  </si>
+  <si>
+    <t>DMA 2, Channel 4</t>
+  </si>
+  <si>
+    <t>SD card RX/TX</t>
+  </si>
+  <si>
+    <t>SD card status interrupts</t>
+  </si>
+  <si>
+    <t>Task scheduler timer (maybe it should have highest priority?)</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -370,7 +391,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
@@ -393,6 +414,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -712,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BA5619-4332-443C-8489-BC42719C7856}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,50 +756,50 @@
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -788,26 +812,26 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -820,7 +844,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,48 +858,48 @@
   <sheetData>
     <row r="1" spans="1:8" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -900,10 +924,10 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -968,34 +992,34 @@
     </row>
     <row r="13" spans="1:8" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1033,11 +1057,11 @@
       <c r="A19" s="6">
         <v>3</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="12" t="s">
         <v>39</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1067,10 +1091,10 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1092,8 +1116,8 @@
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
-        <v>68</v>
+      <c r="E23" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -1106,23 +1130,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFD585D-7293-41F5-9BE9-9477187D65E4}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1130,140 +1161,187 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
+      <c r="C25" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1354,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,16 +1367,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>